<commit_message>
fix be start fe
</commit_message>
<xml_diff>
--- a/database/tb_alternatif.xlsx
+++ b/database/tb_alternatif.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,10 +483,130 @@
         <v>3.5</v>
       </c>
       <c r="E2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F2" t="n">
         <v>3</v>
       </c>
-      <c r="F2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Indosat</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Smartfren</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Telkomsel</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tri</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>